<commit_message>
change added api testing by zip code,city id
</commit_message>
<xml_diff>
--- a/WeatherApi/src/test/resources/DataExcelRead.xlsx
+++ b/WeatherApi/src/test/resources/DataExcelRead.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\WeatherApi\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\WeatherAPI\WeatherApi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBC09A3-E3A1-4B9F-8E62-7027D7EBE2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9984CC-D129-4E2F-B996-59C9CF9389FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28470" yWindow="1740" windowWidth="9675" windowHeight="9165" activeTab="1" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
     <sheet name="WeatherAPITestParameters" sheetId="1" r:id="rId2"/>
+    <sheet name="ZipParameters" sheetId="3" r:id="rId3"/>
+    <sheet name="CityIDParameters" sheetId="4" r:id="rId4"/>
+    <sheet name="CityNameCountryParameters" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>appid</t>
   </si>
@@ -110,6 +113,45 @@
   </si>
   <si>
     <t>TC-010</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Bhilai,IN</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>411027,IN</t>
+  </si>
+  <si>
+    <t>TC-011</t>
+  </si>
+  <si>
+    <t>TC-012</t>
+  </si>
+  <si>
+    <t>TC-013</t>
+  </si>
+  <si>
+    <t>TC-014</t>
+  </si>
+  <si>
+    <t>TC-015</t>
+  </si>
+  <si>
+    <t>TC-016</t>
+  </si>
+  <si>
+    <t>TC-017</t>
   </si>
 </sst>
 </file>
@@ -184,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -210,6 +252,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EFADB9-F0FA-43BE-96E2-38C9DEE830C5}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,4 +838,130 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F93A319-BB03-4D76-B678-6AAAA29B8CC9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FAA6BB6-6EF4-412D-9D0B-4F72D4F5DEB6}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1259229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1261481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846689CD-90C9-40ED-8979-3759F27A5DBE}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Level 2 framework changes
</commit_message>
<xml_diff>
--- a/WeatherApi/src/test/resources/DataExcelRead.xlsx
+++ b/WeatherApi/src/test/resources/DataExcelRead.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\WeatherAPI\WeatherApi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9984CC-D129-4E2F-B996-59C9CF9389FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF72CBD6-F965-41F4-867D-660B0D4ED2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EFADB9-F0FA-43BE-96E2-38C9DEE830C5}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +754,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="2">
-        <v>21.14</v>
+        <v>17.38</v>
       </c>
       <c r="C7" s="2">
         <v>78.48</v>
@@ -922,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846689CD-90C9-40ED-8979-3759F27A5DBE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Asserting values from excel
</commit_message>
<xml_diff>
--- a/WeatherApi/src/test/resources/DataExcelRead.xlsx
+++ b/WeatherApi/src/test/resources/DataExcelRead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\WeatherAPI\WeatherApi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8554209-3105-44AD-8C71-B9E36080528D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DE5BF3-33FB-4500-A010-1275D74D6856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19095" yWindow="2490" windowWidth="16545" windowHeight="11085" firstSheet="4" activeTab="6" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>appid</t>
   </si>
@@ -171,15 +171,6 @@
     <t>US</t>
   </si>
   <si>
-    <t>Aundh Camp</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t> 77.2311</t>
-  </si>
-  <si>
     <t>Houston</t>
   </si>
   <si>
@@ -214,6 +205,12 @@
   </si>
   <si>
     <t>timezone</t>
+  </si>
+  <si>
+    <t>AundhCamp</t>
+  </si>
+  <si>
+    <t>NewDelhi</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B63E30-5AEF-42E7-B7E4-2CF97A00A2FE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,29 +1160,29 @@
         <v>16</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -1205,7 +1202,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>43</v>
@@ -1226,13 +1223,13 @@
         <v>36</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>48</v>
+      <c r="D4" s="12">
+        <v>77.231099999999998</v>
       </c>
       <c r="E4" s="12">
         <v>28.6128</v>
@@ -1272,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E27CA3-F588-4314-AA0E-27D3534607FC}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,22 +1280,22 @@
         <v>16</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1346,7 +1343,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
changes made in excel
</commit_message>
<xml_diff>
--- a/WeatherApi/src/test/resources/DataExcelRead.xlsx
+++ b/WeatherApi/src/test/resources/DataExcelRead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\WeatherAPI\WeatherApi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5F345-46F0-4515-B686-E3D6591B9AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA71B2-DC1F-4E0C-8FDF-709F89FF85C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="6" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
+    <workbookView xWindow="4344" yWindow="2676" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="5" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
@@ -165,52 +165,52 @@
     <t>IN</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>city.name</t>
+  </si>
+  <si>
+    <t>city.country</t>
+  </si>
+  <si>
+    <t>city.coord.lon</t>
+  </si>
+  <si>
+    <t>city.coord.lat</t>
+  </si>
+  <si>
+    <t>city.id</t>
+  </si>
+  <si>
+    <t>city.timezone</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sys.country</t>
+  </si>
+  <si>
+    <t>coord.lon</t>
+  </si>
+  <si>
+    <t>coord.lat</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
     <t>New York</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>city.name</t>
-  </si>
-  <si>
-    <t>city.country</t>
-  </si>
-  <si>
-    <t>city.coord.lon</t>
-  </si>
-  <si>
-    <t>city.coord.lat</t>
-  </si>
-  <si>
-    <t>city.id</t>
-  </si>
-  <si>
-    <t>city.timezone</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>sys.country</t>
-  </si>
-  <si>
-    <t>coord.lon</t>
-  </si>
-  <si>
-    <t>coord.lat</t>
-  </si>
-  <si>
-    <t>timezone</t>
-  </si>
-  <si>
-    <t>AundhCamp</t>
-  </si>
-  <si>
-    <t>NewDelhi</t>
+    <t>Aundh Camp</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B63E30-5AEF-42E7-B7E4-2CF97A00A2FE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,22 +1160,22 @@
         <v>16</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E27CA3-F588-4314-AA0E-27D3534607FC}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,22 +1288,22 @@
         <v>16</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1330,10 +1330,10 @@
         <v>33</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="D3" s="18">
         <v>-73.996700000000004</v>
@@ -1350,10 +1350,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="12">
         <v>-95.363299999999995</v>
@@ -1376,7 +1376,7 @@
         <v>-112.074</v>
       </c>
       <c r="E5" s="19">
-        <v>33.448399999999999</v>
+        <v>33.44838</v>
       </c>
       <c r="F5" s="19">
         <v>5308655</v>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="19">
         <v>-87.65</v>

</xml_diff>

<commit_message>
change in longitude value
</commit_message>
<xml_diff>
--- a/WeatherApi/src/test/resources/DataExcelRead.xlsx
+++ b/WeatherApi/src/test/resources/DataExcelRead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\WeatherAPI\WeatherApi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA71B2-DC1F-4E0C-8FDF-709F89FF85C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2874694-47D0-426F-80CE-2230A1276AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4344" yWindow="2676" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="5" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
+    <workbookView xWindow="4344" yWindow="2676" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="6" xr2:uid="{C7FE4CCB-625E-45F0-ABBD-F363E61153F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
@@ -1142,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B63E30-5AEF-42E7-B7E4-2CF97A00A2FE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E27CA3-F588-4314-AA0E-27D3534607FC}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,7 +1376,7 @@
         <v>-112.074</v>
       </c>
       <c r="E5" s="19">
-        <v>33.44838</v>
+        <v>33.448399999999999</v>
       </c>
       <c r="F5" s="19">
         <v>5308655</v>

</xml_diff>